<commit_message>
need to work on fin analysis
</commit_message>
<xml_diff>
--- a/FinAnalysis.xlsx
+++ b/FinAnalysis.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
@@ -528,79 +528,79 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Apr-24</v>
+        <v>Jan-25</v>
       </c>
       <c r="B2">
-        <v>22021443</v>
+        <v>31266986</v>
       </c>
       <c r="C2">
-        <v>1219263</v>
+        <v>1795766</v>
       </c>
       <c r="D2">
-        <v>3698350</v>
+        <v>3785580</v>
       </c>
       <c r="E2">
-        <v>26939056</v>
+        <v>36848332</v>
       </c>
       <c r="F2">
-        <v>34363</v>
+        <v>78747</v>
       </c>
       <c r="G2">
-        <v>6321474</v>
+        <v>7374490.800000001</v>
       </c>
       <c r="H2" t="str">
-        <v>37%</v>
+        <v>24%</v>
       </c>
       <c r="I2">
-        <v>6068967.0200000005</v>
+        <v>8384726.6</v>
       </c>
       <c r="J2">
-        <v>862790</v>
+        <v>2279115</v>
       </c>
       <c r="K2">
-        <v>13253231.02</v>
+        <v>18038332.4</v>
       </c>
       <c r="L2" t="str">
-        <v>77%</v>
+        <v>58%</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>288446</v>
+        <v>4734</v>
       </c>
       <c r="O2">
-        <v>3591209</v>
+        <v>3813120</v>
       </c>
       <c r="P2">
-        <v>17132886.02</v>
+        <v>21856186.4</v>
       </c>
       <c r="Q2" t="str">
         <v>100%</v>
       </c>
       <c r="R2">
-        <v>878365</v>
+        <v>761934</v>
       </c>
       <c r="S2" t="str">
-        <v>5%</v>
+        <v>3%</v>
       </c>
       <c r="T2">
-        <v>4493331</v>
+        <v>7149303.5</v>
       </c>
       <c r="U2" t="str">
-        <v>26%</v>
+        <v>33%</v>
       </c>
       <c r="V2">
         <v>0</v>
       </c>
       <c r="W2">
-        <v>5371696</v>
+        <v>7911237.5</v>
       </c>
       <c r="X2" t="str">
-        <v>31%</v>
+        <v>36%</v>
       </c>
       <c r="Y2">
-        <v>4468836.98</v>
+        <v>7159655.1000000015</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -615,104 +615,12 @@
         <v>0%</v>
       </c>
       <c r="AD2">
-        <v>4468836.98</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>May-24</v>
-      </c>
-      <c r="B3">
-        <v>26470108</v>
-      </c>
-      <c r="C3">
-        <v>1242959</v>
-      </c>
-      <c r="D3">
-        <v>5235425</v>
-      </c>
-      <c r="E3">
-        <v>32948492</v>
-      </c>
-      <c r="F3">
-        <v>41351</v>
-      </c>
-      <c r="G3">
-        <v>6715975.640000001</v>
-      </c>
-      <c r="H3" t="str">
-        <v>28%</v>
-      </c>
-      <c r="I3">
-        <v>4649643.27</v>
-      </c>
-      <c r="J3">
-        <v>7875384</v>
-      </c>
-      <c r="K3">
-        <v>19241002.91</v>
-      </c>
-      <c r="L3" t="str">
-        <v>79%</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>261104</v>
-      </c>
-      <c r="O3">
-        <v>4899771</v>
-      </c>
-      <c r="P3">
-        <v>24401877.91</v>
-      </c>
-      <c r="Q3" t="str">
-        <v>100%</v>
-      </c>
-      <c r="R3">
-        <v>744437</v>
-      </c>
-      <c r="S3" t="str">
-        <v>3%</v>
-      </c>
-      <c r="T3">
-        <v>564180</v>
-      </c>
-      <c r="U3" t="str">
-        <v>2%</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>1308617</v>
-      </c>
-      <c r="X3" t="str">
-        <v>5%</v>
-      </c>
-      <c r="Y3">
-        <v>7279348.09</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3" t="str">
-        <v>0%</v>
-      </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3" t="str">
-        <v>0%</v>
-      </c>
-      <c r="AD3">
-        <v>7279348.09</v>
+        <v>7159655.1000000015</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AD3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AD2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>